<commit_message>
SELECT Country FROM Customers
</commit_message>
<xml_diff>
--- a/SQL-Basic/SQL Pratice.xlsx
+++ b/SQL-Basic/SQL Pratice.xlsx
@@ -255,7 +255,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +267,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -291,7 +297,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -351,17 +357,11 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -369,23 +369,29 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
@@ -776,7 +782,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="45.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="47.25" customFormat="1" s="4">
       <c r="A9" s="11">
         <v>4</v>
       </c>
@@ -790,7 +796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="45.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="47.25" customFormat="1" s="4">
       <c r="A10" s="11">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Lọc ra những khách hàng thuộc Canada: SELECT DISTINCT Country 'CANADA' FROM Customers;
</commit_message>
<xml_diff>
--- a/SQL-Basic/SQL Pratice.xlsx
+++ b/SQL-Basic/SQL Pratice.xlsx
@@ -255,7 +255,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,7 +271,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -293,12 +293,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -349,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -384,9 +378,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -394,7 +385,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,10 +695,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="60.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="71.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="15" width="45.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="6.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="60.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="71.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="45.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -789,10 +780,10 @@
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -803,7 +794,7 @@
       <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="3"/>
@@ -815,7 +806,7 @@
       <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="3"/>
@@ -854,7 +845,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="32.25" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="33.75" customFormat="1" s="4">
       <c r="A15" s="11">
         <v>10</v>
       </c>
@@ -866,7 +857,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="32.25" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="33.75" customFormat="1" s="4">
       <c r="A16" s="11">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Lọc ra những khách hàng có tên chứa kí tự 'Bo'
</commit_message>
<xml_diff>
--- a/SQL-Basic/SQL Pratice.xlsx
+++ b/SQL-Basic/SQL Pratice.xlsx
@@ -51,9 +51,7 @@
 WHERE CustomerName LIKE 'Bo%';</t>
   </si>
   <si>
-    <t>SELECT column1, column2, ...
-FROM table_name
-WHERE columnN LIKE pattern;</t>
+    <t/>
   </si>
   <si>
     <t>Lọc ra những khách hàng có tên chứa kí tự "Bo"</t>
@@ -343,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -377,6 +375,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -695,10 +696,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="60.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="71.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="45.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="6.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="60.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="71.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="15" width="45.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -783,7 +784,7 @@
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="12" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lấy ra tên khách hàng chưa đăng ký địa chỉ : SELECT * FROM Customers WHERE Address IS Null
</commit_message>
<xml_diff>
--- a/SQL-Basic/SQL Pratice.xlsx
+++ b/SQL-Basic/SQL Pratice.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Thực hành trên trang https://www.w3schools.com/sql/trysql.asp?filename=trysql_select_all</t>
   </si>
@@ -49,9 +49,6 @@
     <t>SELECT CustomerName
 FROM Customers
 WHERE CustomerName LIKE 'Bo%';</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Lọc ra những khách hàng có tên chứa kí tự "Bo"</t>
@@ -341,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -375,9 +372,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -696,10 +690,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="60.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="71.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="15" width="45.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="6.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="60.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="71.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="45.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -784,19 +778,17 @@
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="D9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="47.25" customFormat="1" s="4">
       <c r="A10" s="11">
         <v>5</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="D10" s="3"/>
     </row>
@@ -805,10 +797,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D11" s="3"/>
     </row>
@@ -817,10 +809,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -829,10 +821,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D13" s="3"/>
     </row>
@@ -841,7 +833,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -851,10 +843,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="D15" s="3"/>
     </row>
@@ -863,10 +855,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -875,10 +867,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D17" s="3"/>
     </row>
@@ -887,7 +879,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -897,7 +889,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -907,7 +899,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -917,7 +909,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -927,7 +919,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -937,7 +929,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -947,17 +939,17 @@
         <v>19</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="27.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A25" s="11">
         <v>20</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -967,37 +959,37 @@
         <v>21</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A27" s="11">
         <v>22</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A28" s="11">
         <v>23</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="24.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A29" s="11">
         <v>24</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1007,37 +999,37 @@
         <v>25</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="25.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A31" s="11">
         <v>26</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="25.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5" customFormat="1" s="4">
       <c r="A32" s="11">
         <v>27</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A33" s="11">
         <v>28</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1047,7 +1039,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1057,27 +1049,27 @@
         <v>30</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A36" s="11">
         <v>31</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A37" s="11">
         <v>32</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1087,7 +1079,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1097,7 +1089,7 @@
         <v>25</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1107,27 +1099,27 @@
         <v>26</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="32.25" customFormat="1" s="4">
       <c r="A41" s="11">
         <v>27</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="45.75" customFormat="1" s="4">
       <c r="A42" s="11">
         <v>28</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1137,17 +1129,17 @@
         <v>29</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="45.75" customFormat="1" s="4">
       <c r="A44" s="11">
         <v>30</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1157,7 +1149,7 @@
         <v>25</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1167,7 +1159,7 @@
         <v>26</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1177,7 +1169,7 @@
         <v>27</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -1187,7 +1179,7 @@
         <v>28</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -1197,7 +1189,7 @@
         <v>29</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -1207,7 +1199,7 @@
         <v>25</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>

</xml_diff>